<commit_message>
Fix error mari carmen
</commit_message>
<xml_diff>
--- a/Inherit/bin/Debug/net6.0-windows/Assets/Componentes.xlsx
+++ b/Inherit/bin/Debug/net6.0-windows/Assets/Componentes.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Cuenta 1</t>
+  </si>
+  <si>
+    <t>Cuenta 2</t>
   </si>
 </sst>
 </file>
@@ -400,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -422,6 +428,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0">
+        <v>564856</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0">
+        <v>45200</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>